<commit_message>
Clean up Data Exploration Folder
Deleted some files that I felt were clutter at this point and added some files that I thought would be useful for whoever clones the repo.
</commit_message>
<xml_diff>
--- a/Data Exploration/TOD Statistics.xlsx
+++ b/Data Exploration/TOD Statistics.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,19 +8,29 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\TNC-Demand-Model\Data Exploration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8FD3370D-0077-4AFC-B883-842C804CF066}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE87E289-08C7-43B4-AEAF-DE516F01B383}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="11160"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Trip Miles_stats" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="9">
   <si>
     <t>TOD</t>
   </si>
@@ -48,35 +58,11 @@
   <si>
     <t>Sum per Hour</t>
   </si>
-  <si>
-    <t>1 - 8pm-6am</t>
-  </si>
-  <si>
-    <t>2 - 6am-7am</t>
-  </si>
-  <si>
-    <t>3 - 7am-9am</t>
-  </si>
-  <si>
-    <t>4 - 9am-10am</t>
-  </si>
-  <si>
-    <t>5 - 10am-2pm</t>
-  </si>
-  <si>
-    <t>6 - 2pm-4pm</t>
-  </si>
-  <si>
-    <t>7 - 4pm-6pm</t>
-  </si>
-  <si>
-    <t>8 - 6pm-8pm</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)"/>
@@ -560,15 +546,16 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="20" builtinId="30" customBuiltin="1"/>
@@ -924,41 +911,43 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O22"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:O8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M14" sqref="M14"/>
+      <selection activeCell="B1" sqref="B1:O7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="3" max="5" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="13.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C1" s="4" t="s">
+    <row r="1" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4" t="s">
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4" t="s">
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="L1" s="4"/>
-      <c r="M1" s="4"/>
-      <c r="N1" s="4"/>
-      <c r="O1" s="4"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="5"/>
+      <c r="N1" s="5"/>
+      <c r="O1" s="5"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
@@ -976,16 +965,16 @@
       <c r="F2" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="H2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="I2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="J2" s="4" t="s">
         <v>4</v>
       </c>
       <c r="K2" s="1" t="s">
@@ -1011,19 +1000,19 @@
       <c r="B3">
         <v>1</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="3">
         <v>0</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="3">
         <v>49.8</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="3">
         <v>4.4289435809139297</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="3">
         <v>6976130.8999998998</v>
       </c>
-      <c r="G3" s="5">
+      <c r="G3" s="4">
         <v>0</v>
       </c>
       <c r="H3" s="3">
@@ -1035,21 +1024,21 @@
       <c r="J3" s="3">
         <v>20711513.833333332</v>
       </c>
-      <c r="K3" s="1">
-        <v>1.0000003011459699</v>
+      <c r="K3" s="4">
+        <v>1.0000004193661001</v>
       </c>
       <c r="L3" s="3">
-        <v>76.506679899766695</v>
-      </c>
-      <c r="M3" s="1">
-        <v>1.2932458622792899</v>
+        <v>76.061446476077506</v>
+      </c>
+      <c r="M3" s="3">
+        <v>1.28969335433053</v>
       </c>
       <c r="N3" s="3">
-        <v>162919.23399235899</v>
+        <v>162418.82227097001</v>
       </c>
       <c r="O3" s="2">
         <f>N3/10</f>
-        <v>16291.923399235899</v>
+        <v>16241.882227097001</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
@@ -1059,19 +1048,19 @@
       <c r="B4">
         <v>2</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="3">
         <v>0</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="3">
         <v>48.5</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="3">
         <v>6.5484179275501804</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="3">
         <v>1005810.79999999</v>
       </c>
-      <c r="G4" s="5">
+      <c r="G4" s="4">
         <v>0</v>
       </c>
       <c r="H4" s="3">
@@ -1083,21 +1072,21 @@
       <c r="J4" s="3">
         <v>2864526.25</v>
       </c>
-      <c r="K4" s="1">
-        <v>1.0000001149206099</v>
+      <c r="K4" s="4">
+        <v>1.00000041311336</v>
       </c>
       <c r="L4" s="3">
-        <v>20.4146768917904</v>
-      </c>
-      <c r="M4" s="1">
-        <v>1.10214040628608</v>
+        <v>20.3967835689749</v>
+      </c>
+      <c r="M4" s="3">
+        <v>1.1290802197437699</v>
       </c>
       <c r="N4" s="3">
-        <v>26316.908621299201</v>
+        <v>27111.4742364876</v>
       </c>
       <c r="O4" s="2">
         <f>N4/1</f>
-        <v>26316.908621299201</v>
+        <v>27111.4742364876</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
@@ -1107,19 +1096,19 @@
       <c r="B5">
         <v>3</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="3">
         <v>0</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="3">
         <v>49.5</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="3">
         <v>4.27257789236912</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="3">
         <v>3637395.1000000699</v>
       </c>
-      <c r="G5" s="5">
+      <c r="G5" s="4">
         <v>0</v>
       </c>
       <c r="H5" s="3">
@@ -1131,21 +1120,21 @@
       <c r="J5" s="3">
         <v>16093763.383333333</v>
       </c>
-      <c r="K5" s="1">
-        <v>1.00000047356764</v>
+      <c r="K5" s="4">
+        <v>1.00000008971013</v>
       </c>
       <c r="L5" s="3">
-        <v>189.54691290814901</v>
-      </c>
-      <c r="M5" s="1">
-        <v>1.1982780411951299</v>
+        <v>189.51812437433901</v>
+      </c>
+      <c r="M5" s="3">
+        <v>1.2669113008570101</v>
       </c>
       <c r="N5" s="3">
-        <v>92751.513500668007</v>
+        <v>98469.413947810404</v>
       </c>
       <c r="O5" s="2">
         <f>N5/2</f>
-        <v>46375.756750334003</v>
+        <v>49234.706973905202</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
@@ -1155,19 +1144,19 @@
       <c r="B6">
         <v>4</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="3">
         <v>0</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="3">
         <v>49.8</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="3">
         <v>4.2415548817526201</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="3">
         <v>1675855.29999999</v>
       </c>
-      <c r="G6" s="5">
+      <c r="G6" s="4">
         <v>0</v>
       </c>
       <c r="H6" s="3">
@@ -1179,21 +1168,21 @@
       <c r="J6" s="3">
         <v>6469496.1166666662</v>
       </c>
-      <c r="K6" s="1">
-        <v>1.0000001291054099</v>
+      <c r="K6" s="6">
+        <v>1.0000005587499701</v>
       </c>
       <c r="L6" s="3">
-        <v>81.075971532442495</v>
-      </c>
-      <c r="M6" s="1">
-        <v>1.1242559743865901</v>
+        <v>81.076169843729801</v>
+      </c>
+      <c r="M6" s="3">
+        <v>1.14400052526505</v>
       </c>
       <c r="N6" s="3">
-        <v>59343.851607996199</v>
+        <v>60749.859893150198</v>
       </c>
       <c r="O6" s="2">
         <f>N6/1</f>
-        <v>59343.851607996199</v>
+        <v>60749.859893150198</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
@@ -1203,19 +1192,19 @@
       <c r="B7">
         <v>5</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="3">
         <v>0</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="3">
         <v>49.6</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="3">
         <v>4.84002589065304</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="3">
         <v>5028714.3000001498</v>
       </c>
-      <c r="G7" s="5">
+      <c r="G7" s="4">
         <v>0</v>
       </c>
       <c r="H7" s="3">
@@ -1227,261 +1216,27 @@
       <c r="J7" s="3">
         <v>15573798.083333334</v>
       </c>
-      <c r="K7" s="1">
-        <v>1.0000004943043701</v>
+      <c r="K7" s="4">
+        <v>1.0000000084637499</v>
       </c>
       <c r="L7" s="3">
-        <v>146.86522777105901</v>
-      </c>
-      <c r="M7" s="1">
-        <v>1.22326409405853</v>
+        <v>145.06420275538801</v>
+      </c>
+      <c r="M7" s="3">
+        <v>1.2056465879525999</v>
       </c>
       <c r="N7" s="3">
-        <v>120634.63516377</v>
+        <v>118835.761588136</v>
       </c>
       <c r="O7" s="2">
         <f>N7/4</f>
-        <v>30158.6587909425</v>
+        <v>29708.940397033999</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>5</v>
-      </c>
-      <c r="B8">
-        <v>6</v>
-      </c>
-      <c r="C8">
-        <v>0</v>
-      </c>
-      <c r="D8">
-        <v>49.1</v>
-      </c>
-      <c r="E8">
-        <v>4.9596441188865796</v>
-      </c>
-      <c r="F8">
-        <v>2907378.1000001398</v>
-      </c>
-      <c r="G8" s="5">
-        <v>0</v>
-      </c>
-      <c r="H8" s="3">
-        <v>119.06666666666666</v>
-      </c>
-      <c r="I8" s="1">
-        <v>17.613112831019169</v>
-      </c>
-      <c r="J8" s="3">
-        <v>10324930.033333333</v>
-      </c>
-      <c r="K8" s="1">
-        <v>1.00000011260773</v>
-      </c>
-      <c r="L8" s="3">
-        <v>109.85507035103799</v>
-      </c>
-      <c r="M8" s="1">
-        <v>1.1211750026154499</v>
-      </c>
-      <c r="N8" s="3">
-        <v>100311.527484005</v>
-      </c>
-      <c r="O8" s="2">
-        <f>N8/2</f>
-        <v>50155.763742002498</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>6</v>
-      </c>
-      <c r="B9">
-        <v>7</v>
-      </c>
-      <c r="C9">
-        <v>0</v>
-      </c>
-      <c r="D9">
-        <v>50</v>
-      </c>
-      <c r="E9">
-        <v>4.2150669779610199</v>
-      </c>
-      <c r="F9">
-        <v>3818408.1</v>
-      </c>
-      <c r="G9" s="5">
-        <v>0</v>
-      </c>
-      <c r="H9" s="3">
-        <v>119.91666666666667</v>
-      </c>
-      <c r="I9" s="1">
-        <v>19.148945241998167</v>
-      </c>
-      <c r="J9" s="3">
-        <v>17346933.75</v>
-      </c>
-      <c r="K9" s="1">
-        <v>1.0000000958656301</v>
-      </c>
-      <c r="L9" s="3">
-        <v>88.401704369259207</v>
-      </c>
-      <c r="M9" s="1">
-        <v>1.14876464695853</v>
-      </c>
-      <c r="N9" s="3">
-        <v>124256.12803827001</v>
-      </c>
-      <c r="O9" s="2">
-        <f>N9/2</f>
-        <v>62128.064019135003</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>7</v>
-      </c>
-      <c r="B10">
-        <v>8</v>
-      </c>
-      <c r="C10">
-        <v>0</v>
-      </c>
-      <c r="D10">
-        <v>49.7</v>
-      </c>
-      <c r="E10">
-        <v>3.84546814301045</v>
-      </c>
-      <c r="F10">
-        <v>4244658.5000000801</v>
-      </c>
-      <c r="G10" s="5">
-        <v>0</v>
-      </c>
-      <c r="H10" s="3">
-        <v>119.31666666666666</v>
-      </c>
-      <c r="I10" s="1">
-        <v>15.332141821766101</v>
-      </c>
-      <c r="J10" s="3">
-        <v>16923740.800000001</v>
-      </c>
-      <c r="K10" s="1">
-        <v>1.00000004889646</v>
-      </c>
-      <c r="L10" s="3">
-        <v>98.900718199713197</v>
-      </c>
-      <c r="M10" s="1">
-        <v>1.1827618845136501</v>
-      </c>
-      <c r="N10" s="3">
-        <v>129377.59149941</v>
-      </c>
-      <c r="O10" s="2">
-        <f>N10/2</f>
-        <v>64688.795749705001</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="I11" s="5"/>
-      <c r="J11" s="5"/>
-      <c r="K11" s="5"/>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="H12" s="5"/>
-      <c r="I12" s="5"/>
-      <c r="J12" s="5"/>
-      <c r="K12" s="5"/>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="H13" s="5"/>
-      <c r="I13" s="5"/>
-      <c r="J13" s="5"/>
-      <c r="K13" s="5"/>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="H14" s="5"/>
-      <c r="I14" s="5"/>
-      <c r="J14" s="5"/>
-      <c r="K14" s="5"/>
-      <c r="N14" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="H15" s="5"/>
-      <c r="I15" s="5"/>
-      <c r="J15" s="5"/>
-      <c r="K15" s="5"/>
-      <c r="N15" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="H16" s="5"/>
-      <c r="I16" s="5"/>
-      <c r="J16" s="5"/>
-      <c r="K16" s="5"/>
-      <c r="N16" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="17" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="H17" s="5"/>
-      <c r="I17" s="5"/>
-      <c r="J17" s="5"/>
-      <c r="K17" s="5"/>
-      <c r="N17" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="18" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="H18" s="5"/>
-      <c r="I18" s="5"/>
-      <c r="J18" s="5"/>
-      <c r="K18" s="5"/>
-      <c r="N18" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="19" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="H19" s="5"/>
-      <c r="I19" s="5"/>
-      <c r="J19" s="5"/>
-      <c r="K19" s="5"/>
-      <c r="N19" s="5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="20" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="H20" s="5"/>
-      <c r="I20" s="5"/>
-      <c r="J20" s="5"/>
-      <c r="K20" s="5"/>
-      <c r="N20" s="5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="21" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="H21" s="5"/>
-      <c r="I21" s="5"/>
-      <c r="J21" s="5"/>
-      <c r="K21" s="5"/>
-      <c r="N21" s="5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="22" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="H22" s="5"/>
-      <c r="I22" s="5"/>
-      <c r="J22" s="5"/>
-      <c r="K22" s="5"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>